<commit_message>
Issues with inconsistency fixed
</commit_message>
<xml_diff>
--- a/ClassInteractions.xlsx
+++ b/ClassInteractions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://angecocz-my.sharepoint.com/personal/ondrej_zubec_angeco_cz/Documents/Vyuka/UHK/KIT-KOSW - Ontologie a semanticky web/SeminarniPrace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="8_{91520A85-57E4-47F2-B177-B88665B95AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0C043BB-D06F-4D54-8027-3395FEA2B453}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="8_{91520A85-57E4-47F2-B177-B88665B95AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B952E6D2-6BC6-4952-8F17-E0CB0B9FA127}"/>
   <bookViews>
-    <workbookView xWindow="14205" yWindow="2655" windowWidth="13095" windowHeight="11040" xr2:uid="{BCD4BF20-FBED-41C2-824A-F79744077ED9}"/>
+    <workbookView xWindow="13320" yWindow="1740" windowWidth="13095" windowHeight="11040" xr2:uid="{BCD4BF20-FBED-41C2-824A-F79744077ED9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,9 +80,6 @@
     <t>jeVekovouKategoriiPro</t>
   </si>
   <si>
-    <t>jeMístemPouzitiPro</t>
-  </si>
-  <si>
     <t>jePatentovan</t>
   </si>
   <si>
@@ -125,10 +122,13 @@
     <t>skladaSeZ</t>
   </si>
   <si>
-    <t>jeObdobímPouzitiPro</t>
-  </si>
-  <si>
     <t>jePouzivanJako</t>
+  </si>
+  <si>
+    <t>jeObdobimPouzitiPro</t>
+  </si>
+  <si>
+    <t>jeMistemPouzitiPro</t>
   </si>
 </sst>
 </file>
@@ -496,7 +496,7 @@
   <dimension ref="A5:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,10 +526,10 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>29</v>
@@ -543,7 +543,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -557,10 +557,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -571,10 +571,10 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -585,10 +585,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -599,10 +599,10 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
         <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -613,7 +613,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
@@ -627,18 +627,18 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>